<commit_message>
Piwik-Analyse Seitenaufrufe 2. Ebene fertiggestellt
</commit_message>
<xml_diff>
--- a/Piwik-Analyse/Seitenaufrufe.xlsx
+++ b/Piwik-Analyse/Seitenaufrufe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="560" windowWidth="24600" windowHeight="21140"/>
+    <workbookView xWindow="14660" yWindow="460" windowWidth="23740" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="271">
   <si>
     <t xml:space="preserve">Ebene </t>
   </si>
@@ -1539,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F171" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="J206" sqref="J206"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="L218" sqref="L218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6655,9 +6655,15 @@
       <c r="I206" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J206" s="3"/>
-      <c r="K206" s="3"/>
-      <c r="L206" s="14"/>
+      <c r="J206" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="K206" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="L206" s="14" t="s">
+        <v>214</v>
+      </c>
       <c r="M206" s="3"/>
       <c r="N206" s="3"/>
       <c r="O206" s="3">

</xml_diff>